<commit_message>
This might be wild, but I'm committing all of these.
</commit_message>
<xml_diff>
--- a/subnational maps/TBSubnational/Data/KHM.xlsx
+++ b/subnational maps/TBSubnational/Data/KHM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
   <si>
     <t>Country</t>
   </si>
@@ -113,13 +113,16 @@
   </si>
   <si>
     <t>Takêv</t>
+  </si>
+  <si>
+    <t>Rate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -159,6 +162,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -184,7 +193,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -199,11 +208,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,9 +537,10 @@
     <col min="4" max="4" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="23.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="23.7109375" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -548,8 +565,11 @@
       <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I1" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -565,16 +585,21 @@
       <c r="E2" s="6">
         <v>2803</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="9">
         <v>6778</v>
       </c>
       <c r="G2" s="3">
         <v>713</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="8"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H2" s="13">
+        <f>I2*G2</f>
+        <v>641.70000000000005</v>
+      </c>
+      <c r="I2" s="12">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -590,17 +615,21 @@
       <c r="E3" s="6">
         <v>2653</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="9">
         <v>8247</v>
       </c>
       <c r="G3" s="3">
         <v>908</v>
       </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H3" s="13">
+        <f t="shared" ref="H3:H25" si="0">I3*G3</f>
+        <v>817.2</v>
+      </c>
+      <c r="I3" s="12">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -616,17 +645,21 @@
       <c r="E4" s="6">
         <v>4894</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="9">
         <v>33637</v>
       </c>
       <c r="G4" s="3">
         <v>1935</v>
       </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H4" s="13">
+        <f t="shared" si="0"/>
+        <v>1586.6999999999998</v>
+      </c>
+      <c r="I4" s="12">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -642,17 +675,21 @@
       <c r="E5" s="6">
         <v>1012</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="9">
         <v>4848</v>
       </c>
       <c r="G5" s="3">
         <v>662</v>
       </c>
-      <c r="H5" s="3"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H5" s="13">
+        <f t="shared" si="0"/>
+        <v>622.28</v>
+      </c>
+      <c r="I5" s="12">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -668,17 +705,21 @@
       <c r="E6" s="6">
         <v>2368</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="8">
         <v>6277</v>
       </c>
       <c r="G6" s="3">
         <v>995</v>
       </c>
-      <c r="H6" s="3"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="3"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H6" s="13">
+        <f t="shared" si="0"/>
+        <v>945.25</v>
+      </c>
+      <c r="I6" s="12">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -694,17 +735,21 @@
       <c r="E7" s="6">
         <v>1468</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="8">
         <v>5753</v>
       </c>
       <c r="G7" s="3">
         <v>992</v>
       </c>
-      <c r="H7" s="3"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H7" s="13">
+        <f t="shared" si="0"/>
+        <v>892.80000000000007</v>
+      </c>
+      <c r="I7" s="12">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -720,17 +765,21 @@
       <c r="E8" s="6">
         <v>1342</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="8">
         <v>6338</v>
       </c>
       <c r="G8" s="3">
         <v>631</v>
       </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="3"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H8" s="13">
+        <f t="shared" si="0"/>
+        <v>605.76</v>
+      </c>
+      <c r="I8" s="12">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -746,17 +795,21 @@
       <c r="E9" s="6">
         <v>2995</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="8">
         <v>9320</v>
       </c>
       <c r="G9" s="3">
         <v>1200</v>
       </c>
-      <c r="H9" s="3"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="3"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H9" s="13">
+        <f t="shared" si="0"/>
+        <v>1068</v>
+      </c>
+      <c r="I9" s="12">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -772,17 +825,21 @@
       <c r="E10" s="6">
         <v>171</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="8">
         <v>1214</v>
       </c>
       <c r="G10" s="3">
         <v>94</v>
       </c>
-      <c r="H10" s="3"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H10" s="13">
+        <f t="shared" si="0"/>
+        <v>69.56</v>
+      </c>
+      <c r="I10" s="12">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -798,17 +855,21 @@
       <c r="E11" s="6">
         <v>68</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="8">
         <v>190</v>
       </c>
       <c r="G11" s="3">
         <v>46</v>
       </c>
-      <c r="H11" s="3"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="3"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H11" s="13">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="I11" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -824,17 +885,21 @@
       <c r="E12" s="6">
         <v>456</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="9">
         <v>1129</v>
       </c>
       <c r="G12" s="3">
         <v>186</v>
       </c>
-      <c r="H12" s="3"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="3"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H12" s="13">
+        <f t="shared" si="0"/>
+        <v>154.38</v>
+      </c>
+      <c r="I12" s="12">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -850,17 +915,21 @@
       <c r="E13" s="6">
         <v>170</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="8">
         <v>354</v>
       </c>
       <c r="G13" s="3">
         <v>90</v>
       </c>
-      <c r="H13" s="3"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="3"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H13" s="13">
+        <f t="shared" si="0"/>
+        <v>77.400000000000006</v>
+      </c>
+      <c r="I13" s="12">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -876,17 +945,21 @@
       <c r="E14" s="6">
         <v>417</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="8">
         <v>1226</v>
       </c>
       <c r="G14" s="3">
         <v>189</v>
       </c>
-      <c r="H14" s="3"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="3"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H14" s="13">
+        <f t="shared" si="0"/>
+        <v>156.87</v>
+      </c>
+      <c r="I14" s="12">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -902,17 +975,21 @@
       <c r="E15" s="6">
         <v>34</v>
       </c>
-      <c r="F15" s="10">
+      <c r="F15" s="9">
         <v>481</v>
       </c>
       <c r="G15" s="3">
         <v>37</v>
       </c>
-      <c r="H15" s="3"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="3"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H15" s="13">
+        <f t="shared" si="0"/>
+        <v>22.57</v>
+      </c>
+      <c r="I15" s="12">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -928,17 +1005,21 @@
       <c r="E16" s="6">
         <v>448</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F16" s="9">
         <v>1710</v>
       </c>
       <c r="G16" s="3">
         <v>328</v>
       </c>
-      <c r="H16" s="3"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="3"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H16" s="13">
+        <f t="shared" si="0"/>
+        <v>288.64</v>
+      </c>
+      <c r="I16" s="12">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -954,17 +1035,21 @@
       <c r="E17" s="6">
         <v>3618</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="8">
         <v>21566</v>
       </c>
       <c r="G17" s="3">
         <v>1260</v>
       </c>
-      <c r="H17" s="3"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="3"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H17" s="13">
+        <f t="shared" si="0"/>
+        <v>1121.4000000000001</v>
+      </c>
+      <c r="I17" s="12">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -980,17 +1065,21 @@
       <c r="E18" s="6">
         <v>1164</v>
       </c>
-      <c r="F18" s="10">
+      <c r="F18" s="9">
         <v>3910</v>
       </c>
       <c r="G18" s="3">
         <v>518</v>
       </c>
-      <c r="H18" s="3"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="3"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H18" s="13">
+        <f t="shared" si="0"/>
+        <v>486.91999999999996</v>
+      </c>
+      <c r="I18" s="12">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1006,17 +1095,21 @@
       <c r="E19" s="6">
         <v>403</v>
       </c>
-      <c r="F19" s="10">
+      <c r="F19" s="9">
         <v>1459</v>
       </c>
       <c r="G19" s="3">
         <v>189</v>
       </c>
-      <c r="H19" s="3"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="3"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H19" s="13">
+        <f t="shared" si="0"/>
+        <v>173.88</v>
+      </c>
+      <c r="I19" s="12">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -1032,17 +1125,21 @@
       <c r="E20" s="6">
         <v>4193</v>
       </c>
-      <c r="F20" s="10">
+      <c r="F20" s="9">
         <v>22916</v>
       </c>
       <c r="G20" s="3">
         <v>1441</v>
       </c>
-      <c r="H20" s="3"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="3"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H20" s="13">
+        <f t="shared" si="0"/>
+        <v>1383.36</v>
+      </c>
+      <c r="I20" s="12">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -1058,17 +1155,21 @@
       <c r="E21" s="6">
         <v>150</v>
       </c>
-      <c r="F21" s="10">
+      <c r="F21" s="9">
         <v>1439</v>
       </c>
       <c r="G21" s="3">
         <v>77</v>
       </c>
-      <c r="H21" s="3"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="3"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H21" s="13">
+        <f t="shared" si="0"/>
+        <v>43.889999999999993</v>
+      </c>
+      <c r="I21" s="12">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -1084,17 +1185,21 @@
       <c r="E22" s="6">
         <v>3329</v>
       </c>
-      <c r="F22" s="10">
+      <c r="F22" s="9">
         <v>13189</v>
       </c>
       <c r="G22" s="3">
         <v>1368</v>
       </c>
-      <c r="H22" s="3"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="3"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H22" s="13">
+        <f t="shared" si="0"/>
+        <v>1203.8399999999999</v>
+      </c>
+      <c r="I22" s="12">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1110,17 +1215,21 @@
       <c r="E23" s="6">
         <v>258</v>
       </c>
-      <c r="F23" s="10">
+      <c r="F23" s="9">
         <v>1399</v>
       </c>
       <c r="G23" s="3">
         <v>127</v>
       </c>
-      <c r="H23" s="3"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="3"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H23" s="13">
+        <f t="shared" si="0"/>
+        <v>118.11</v>
+      </c>
+      <c r="I23" s="12">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1136,17 +1245,21 @@
       <c r="E24" s="6">
         <v>1954</v>
       </c>
-      <c r="F24" s="10">
+      <c r="F24" s="9">
         <v>5607</v>
       </c>
       <c r="G24" s="3">
         <v>763</v>
       </c>
-      <c r="H24" s="3"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="3"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H24" s="13">
+        <f t="shared" si="0"/>
+        <v>732.48</v>
+      </c>
+      <c r="I24" s="12">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -1162,15 +1275,19 @@
       <c r="E25" s="6">
         <v>2715</v>
       </c>
-      <c r="F25" s="10">
+      <c r="F25" s="9">
         <v>14642</v>
       </c>
       <c r="G25" s="3">
         <v>1063</v>
       </c>
-      <c r="H25" s="3"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="3"/>
+      <c r="H25" s="13">
+        <f t="shared" si="0"/>
+        <v>935.44</v>
+      </c>
+      <c r="I25" s="12">
+        <v>0.88</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>